<commit_message>
T-test and visualisation update.
Introduction of more robust t-test scripts and organising of histogram/bar graph scripts.
</commit_message>
<xml_diff>
--- a/Averaged_Sleep_Data.xlsx
+++ b/Averaged_Sleep_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgeannas/Documents/GitHub/FALAH-MATLAB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF41FC8-55A5-AA41-8143-BCD501B32C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92EFE42-9D94-C64E-9BB4-A8E568418D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,9 +538,6 @@
     <t>01:55:12</t>
   </si>
   <si>
-    <t>12:51:27</t>
-  </si>
-  <si>
     <t>01:41:27</t>
   </si>
   <si>
@@ -886,33 +883,18 @@
     <t>02:31:15</t>
   </si>
   <si>
-    <t>08:51:47</t>
-  </si>
-  <si>
-    <t>05:35:39</t>
-  </si>
-  <si>
-    <t>05:27:33</t>
-  </si>
-  <si>
     <t>02:30:57</t>
   </si>
   <si>
     <t>01:25:51</t>
   </si>
   <si>
-    <t>05:23:09</t>
-  </si>
-  <si>
     <t>01:07:42</t>
   </si>
   <si>
     <t>02:03:34</t>
   </si>
   <si>
-    <t>05:57:33</t>
-  </si>
-  <si>
     <t>01:51:21</t>
   </si>
   <si>
@@ -976,9 +958,6 @@
     <t>03:17:12</t>
   </si>
   <si>
-    <t>06:58:42</t>
-  </si>
-  <si>
     <t>01:40:07</t>
   </si>
   <si>
@@ -1163,6 +1142,27 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>00:51:27</t>
+  </si>
+  <si>
+    <t>00:51:47</t>
+  </si>
+  <si>
+    <t>00:35:39</t>
+  </si>
+  <si>
+    <t>02:27:33</t>
+  </si>
+  <si>
+    <t>00:23:09</t>
+  </si>
+  <si>
+    <t>00:57:33</t>
+  </si>
+  <si>
+    <t>03:58:42</t>
   </si>
 </sst>
 </file>
@@ -1211,8 +1211,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1550,7 +1550,7 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1583,7 +1583,7 @@
       <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>64</v>
       </c>
       <c r="G1" t="s">
@@ -1595,11 +1595,11 @@
       <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>68</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1630,19 +1630,19 @@
         <v>153</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="I3">
         <v>8.1419444444444444</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>378</v>
+        <v>358</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1653,7 +1653,7 @@
         <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>111</v>
@@ -1665,19 +1665,19 @@
         <v>154</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I4">
         <v>8.2152777777777786</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>378</v>
+        <v>282</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1700,19 +1700,19 @@
         <v>155</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I5">
         <v>8.3152777777777764</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>378</v>
+        <v>283</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1735,19 +1735,19 @@
         <v>156</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I6">
         <v>9.1552777777777781</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>378</v>
+        <v>359</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1770,10 +1770,10 @@
         <v>157</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I7">
         <v>7.8152777777777782</v>
@@ -1781,8 +1781,8 @@
       <c r="J7" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>378</v>
+      <c r="K7" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1796,7 +1796,7 @@
         <v>73</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E8">
         <v>8.3819444444444446</v>
@@ -1805,19 +1805,19 @@
         <v>158</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I8">
         <v>6.6152777777777789</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>378</v>
+        <v>284</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1828,7 +1828,7 @@
         <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>115</v>
@@ -1840,19 +1840,19 @@
         <v>159</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I9">
         <v>9.0986111111111114</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>378</v>
+        <v>360</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1872,22 +1872,22 @@
         <v>9.1236111111111118</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I10">
         <v>9.6819444444444436</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>378</v>
+        <v>285</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1910,19 +1910,19 @@
         <v>160</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I11">
         <v>7.4219444444444447</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>378</v>
+        <v>286</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1947,8 +1947,8 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="4" t="s">
-        <v>378</v>
+      <c r="K12" s="3" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1962,7 +1962,7 @@
         <v>77</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="E13">
         <v>10.473611111111111</v>
@@ -1971,7 +1971,7 @@
         <v>162</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>144</v>
@@ -1980,10 +1980,10 @@
         <v>9.4152777777777779</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>378</v>
+        <v>174</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -2003,19 +2003,19 @@
         <v>163</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="I14">
         <v>7.9708333333333323</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>378</v>
+      <c r="J14" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -2038,19 +2038,19 @@
         <v>164</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I15">
         <v>9.1886111111111113</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>378</v>
+      <c r="J15" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -2073,19 +2073,19 @@
         <v>165</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I16">
         <v>7.571944444444445</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>378</v>
+      <c r="J16" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -2108,19 +2108,19 @@
         <v>166</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I17">
         <v>7.7119444444444456</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>378</v>
+        <v>287</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -2143,19 +2143,19 @@
         <v>167</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="I18">
         <v>8.6519444444444442</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>378</v>
+        <v>361</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -2181,16 +2181,16 @@
         <v>71</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I19">
         <v>9.3286111111111119</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>378</v>
+        <v>288</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -2201,7 +2201,7 @@
         <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>125</v>
@@ -2210,22 +2210,22 @@
         <v>7.7652777777777775</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I20">
         <v>9.5186111111111096</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="K20" s="3" t="s">
+      <c r="J20" s="4" t="s">
         <v>378</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -2248,19 +2248,19 @@
         <v>169</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="I21">
         <v>8.2236111111111114</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>378</v>
+        <v>289</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -2283,19 +2283,19 @@
         <v>170</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="I22">
         <v>9.5444444444444443</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>378</v>
+        <v>290</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -2318,19 +2318,19 @@
         <v>171</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I23">
         <v>6.9719444444444436</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>378</v>
+      <c r="J23" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -2349,23 +2349,23 @@
       <c r="E24">
         <v>9.781944444444445</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>172</v>
+      <c r="F24" s="4" t="s">
+        <v>374</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I24">
         <v>7.9252777777777768</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>378</v>
+        <v>291</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -2385,22 +2385,22 @@
         <v>10.648611111111112</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I25">
         <v>7.908611111111111</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>378</v>
+        <v>292</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -2420,22 +2420,22 @@
         <v>8.2402777777777771</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I26">
         <v>8.4419444444444451</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>378</v>
+        <v>293</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -2455,22 +2455,22 @@
         <v>9.6819444444444436</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="I27">
         <v>9.2686111111111096</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>378</v>
+        <v>362</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -2487,22 +2487,22 @@
         <v>10.715277777777779</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I28">
         <v>7.8986111111111112</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>378</v>
+        <v>363</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -2525,19 +2525,19 @@
         <v>171</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I29">
         <v>8.8736111111111118</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>378</v>
+        <v>294</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -2557,22 +2557,22 @@
         <v>8.8236111111111111</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I30">
         <v>8.7097222222222204</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>378</v>
+        <v>295</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -2586,28 +2586,28 @@
         <v>94</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E31">
         <v>8.6402777777777775</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I31">
         <v>7.8186111111111103</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>378</v>
+        <v>296</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -2618,28 +2618,28 @@
         <v>95</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="E32">
         <v>10.061111111111112</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I32">
         <v>10.038611111111111</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>378</v>
+        <v>297</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -2659,22 +2659,22 @@
         <v>9.4736111111111114</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I33">
         <v>8.0752777777777762</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>378</v>
+        <v>298</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -2694,22 +2694,22 @@
         <v>7.6902777777777782</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I34">
         <v>9.1852777777777774</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>378</v>
+        <v>364</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -2729,22 +2729,22 @@
         <v>9.7736111111111121</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="I35">
         <v>7.578611111111111</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>378</v>
+        <v>365</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -2752,7 +2752,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>138</v>
@@ -2761,22 +2761,22 @@
         <v>9.2736111111111104</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I36">
         <v>6.9919444444444441</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>378</v>
+        <v>299</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -2787,7 +2787,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>132</v>
@@ -2796,22 +2796,22 @@
         <v>8.87361111111111</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="I37">
         <v>9.5686111111111103</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>378</v>
+        <v>300</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -2831,22 +2831,22 @@
         <v>12.134722222222223</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I38">
         <v>8.6708333333333325</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>378</v>
+        <v>301</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2866,22 +2866,22 @@
         <v>9.6958333333333329</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I39">
         <v>7.9313888888888897</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>378</v>
+        <v>302</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2901,22 +2901,22 @@
         <v>10.640277777777778</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I40">
         <v>8.7861111111111114</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>379</v>
+        <v>303</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2927,31 +2927,31 @@
         <v>58</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="E41">
         <v>9.5486111111111107</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I41">
         <v>10.731944444444444</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>379</v>
+        <v>304</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2971,22 +2971,22 @@
         <v>7.5486111111111107</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I42">
         <v>7.3486111111111114</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>379</v>
+        <v>305</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -3006,22 +3006,22 @@
         <v>9.9819444444444443</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I43">
         <v>7.2777777777777777</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>379</v>
+        <v>306</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -3035,19 +3035,19 @@
       <c r="D44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I44">
         <v>6.5819444444444448</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>379</v>
+        <v>307</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -3067,22 +3067,22 @@
         <v>9.0736111111111111</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I45">
         <v>8.4611111111111121</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>379</v>
+        <v>308</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -3093,7 +3093,7 @@
         <v>59</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>145</v>
@@ -3102,22 +3102,22 @@
         <v>7.6902777777777782</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I46">
         <v>8.6375000000000011</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>379</v>
+        <v>309</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -3131,16 +3131,16 @@
         <v>104</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="E47">
         <v>8.8319444444444457</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>119</v>
@@ -3149,10 +3149,10 @@
         <v>8.6902777777777764</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>379</v>
+        <v>310</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -3163,7 +3163,7 @@
         <v>60</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>146</v>
@@ -3172,22 +3172,22 @@
         <v>6.7736111111111112</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I48">
         <v>8.0208333333333339</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>379</v>
+        <v>366</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -3207,22 +3207,22 @@
         <v>9.7652777777777775</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I49">
         <v>11.62361111111111</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>379</v>
+        <v>311</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -3242,22 +3242,22 @@
         <v>7.4486111111111111</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I50">
         <v>6.5652777777777782</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>379</v>
+      <c r="J50" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -3268,7 +3268,7 @@
         <v>60</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>110</v>
@@ -3277,22 +3277,22 @@
         <v>10.090277777777779</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I51">
         <v>10.104166666666666</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>379</v>
+        <v>312</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -3312,22 +3312,22 @@
         <v>7.8486111111111114</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I52">
         <v>7.7777777777777786</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>379</v>
+        <v>313</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -3341,19 +3341,19 @@
       <c r="D53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I53">
         <v>8.7597222222222211</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>379</v>
+        <v>314</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -3364,7 +3364,7 @@
         <v>58</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>150</v>
@@ -3373,22 +3373,22 @@
         <v>7.5402777777777779</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I54">
         <v>7.8611111111111098</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>379</v>
+        <v>315</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -3408,22 +3408,22 @@
         <v>7.5319444444444441</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I55">
         <v>7.9736111111111105</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>379</v>
+        <v>316</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -3443,22 +3443,22 @@
         <v>8.0069444444444446</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I56">
         <v>6.7111111111111112</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="K56" s="3" t="s">
-        <v>379</v>
+        <v>317</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -3478,22 +3478,22 @@
         <v>9.1652777777777779</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I57">
         <v>7.615277777777778</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="K57" s="3" t="s">
-        <v>379</v>
+        <v>367</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -3513,27 +3513,27 @@
         <v>8.281944444444445</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I58">
         <v>7.3069444444444445</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="K58" s="3" t="s">
-        <v>379</v>
+        <v>299</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="65" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J65" s="2" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>